<commit_message>
refactored mo_jobs for improved readability
</commit_message>
<xml_diff>
--- a/results_tables/all_results_tables.xlsx
+++ b/results_tables/all_results_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1956201e8a4bb6a5/Memory Stick Copy/USB Drive/Imperial/Dissertation/results_tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\OneDrive\Memory Stick Copy\USB Drive\Imperial\Dissertation\results_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{C43D87B0-7851-401C-9051-398CCA02932B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C0751C9-5C5D-41C0-A451-88C856DC2D2F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1517DDA-8B2E-44D1-9EED-047ED422D1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{918A9FAB-82C6-4D12-8E12-7D56407DAB5C}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" firstSheet="5" activeTab="6" xr2:uid="{918A9FAB-82C6-4D12-8E12-7D56407DAB5C}"/>
   </bookViews>
   <sheets>
     <sheet name="doses_results" sheetId="1" r:id="rId1"/>
@@ -478,9 +478,6 @@
     <t>Mean Population Density</t>
   </si>
   <si>
-    <t>Number of Jobs</t>
-  </si>
-  <si>
     <t>DWP Winter Grant Per Capita</t>
   </si>
   <si>
@@ -576,6 +573,9 @@
   <si>
     <t>Primary Care Funding Per Capita</t>
   </si>
+  <si>
+    <t>Estimated Job Counts</t>
+  </si>
 </sst>
 </file>
 
@@ -646,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -656,8 +656,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2339,7 +2338,7 @@
         <v>omicron_support_fund_percapita</v>
       </c>
       <c r="R30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -10918,10 +10917,10 @@
         <v>249</v>
       </c>
       <c r="B250" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C250" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D250">
         <v>0.21681976869461</v>
@@ -11659,10 +11658,10 @@
         <v>268</v>
       </c>
       <c r="B269" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C269" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D269">
         <v>0.13898513205387</v>
@@ -11893,7 +11892,7 @@
         <v>274</v>
       </c>
       <c r="B275" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C275" t="s">
         <v>109</v>
@@ -12322,7 +12321,7 @@
         <v>285</v>
       </c>
       <c r="B286" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C286" t="s">
         <v>97</v>
@@ -12400,10 +12399,10 @@
         <v>287</v>
       </c>
       <c r="B288" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C288" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D288">
         <v>0.17223178943780701</v>
@@ -12517,7 +12516,7 @@
         <v>290</v>
       </c>
       <c r="B291" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C291" t="s">
         <v>96</v>
@@ -12595,7 +12594,7 @@
         <v>292</v>
       </c>
       <c r="B293" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C293" t="s">
         <v>98</v>
@@ -12634,7 +12633,7 @@
         <v>293</v>
       </c>
       <c r="B294" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C294" t="s">
         <v>109</v>
@@ -12751,7 +12750,7 @@
         <v>296</v>
       </c>
       <c r="B297" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C297" t="s">
         <v>105</v>
@@ -15106,8 +15105,8 @@
   </sheetPr>
   <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:J35"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15604,7 +15603,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="2" t="str" cm="1">
         <f t="array" ref="C10">_xlfn.XLOOKUP($A10&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -15963,41 +15962,41 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="9" t="str" cm="1">
+      <c r="C19" s="8" t="str" cm="1">
         <f t="array" ref="C19">_xlfn.XLOOKUP($A19&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v>-0.67[-1.04,-0.29]</v>
       </c>
-      <c r="D19" s="9" t="str" cm="1">
+      <c r="D19" s="8" t="str" cm="1">
         <f t="array" ref="D19">_xlfn.XLOOKUP($A19&amp;D$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v>-0.55[-0.94,-0.16]</v>
       </c>
-      <c r="E19" s="9" t="str" cm="1">
+      <c r="E19" s="8" t="str" cm="1">
         <f t="array" ref="E19">_xlfn.XLOOKUP($A19&amp;E$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v/>
       </c>
-      <c r="F19" s="9" t="str" cm="1">
+      <c r="F19" s="8" t="str" cm="1">
         <f t="array" ref="F19">_xlfn.XLOOKUP($A19&amp;F$3&amp;$F$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v>-0.42[-0.74,-0.11]</v>
       </c>
-      <c r="G19" s="9" t="str" cm="1">
+      <c r="G19" s="8" t="str" cm="1">
         <f t="array" ref="G19">_xlfn.XLOOKUP($A19&amp;G$3&amp;$F$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v>-0.36[-0.71,-0.02]</v>
       </c>
-      <c r="H19" s="9" t="str" cm="1">
+      <c r="H19" s="8" t="str" cm="1">
         <f t="array" ref="H19">_xlfn.XLOOKUP($A19&amp;H$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v/>
       </c>
-      <c r="I19" s="9" t="str" cm="1">
+      <c r="I19" s="8" t="str" cm="1">
         <f t="array" ref="I19">_xlfn.XLOOKUP($A19&amp;I$3&amp;$I$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v>-0.64[-1.06,-0.23]</v>
       </c>
-      <c r="J19" s="9" t="str" cm="1">
+      <c r="J19" s="8" t="str" cm="1">
         <f t="array" ref="J19">_xlfn.XLOOKUP($A19&amp;J$3&amp;$I$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v/>
       </c>
@@ -16367,7 +16366,7 @@
         <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C29" t="str" cm="1">
         <f t="array" ref="C29">_xlfn.XLOOKUP($A29&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -16404,10 +16403,10 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C30" t="str" cm="1">
         <f t="array" ref="C30">_xlfn.XLOOKUP($A30&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -16487,7 +16486,7 @@
         <v>98</v>
       </c>
       <c r="B32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C32" t="str" cm="1">
         <f t="array" ref="C32">_xlfn.XLOOKUP($A32&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -16527,7 +16526,7 @@
         <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C33" t="str" cm="1">
         <f t="array" ref="C33">_xlfn.XLOOKUP($A33&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -16567,7 +16566,7 @@
         <v>105</v>
       </c>
       <c r="B34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C34" t="str" cm="1">
         <f t="array" ref="C34">_xlfn.XLOOKUP($A34&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -16607,7 +16606,7 @@
         <v>107</v>
       </c>
       <c r="B35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C35" t="str" cm="1">
         <f t="array" ref="C35">_xlfn.XLOOKUP($A35&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -16656,7 +16655,7 @@
   <dimension ref="A1:O313"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="105" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:J35"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16980,7 +16979,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="2" t="str" cm="1">
         <f t="array" ref="C10">_xlfn.XLOOKUP($A10&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -17344,46 +17343,46 @@
       </c>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="9" t="str" cm="1">
+      <c r="C19" s="8" t="str" cm="1">
         <f t="array" ref="C19">_xlfn.XLOOKUP($A19&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v>-0.62[-1.00,-0.24]</v>
       </c>
-      <c r="D19" s="9" t="str" cm="1">
+      <c r="D19" s="8" t="str" cm="1">
         <f t="array" ref="D19">_xlfn.XLOOKUP($A19&amp;D$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v>-0.52[-0.92,-0.13]</v>
       </c>
-      <c r="E19" s="9" t="str" cm="1">
+      <c r="E19" s="8" t="str" cm="1">
         <f t="array" ref="E19">_xlfn.XLOOKUP($A19&amp;E$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v/>
       </c>
-      <c r="F19" s="9" t="str" cm="1">
+      <c r="F19" s="8" t="str" cm="1">
         <f t="array" ref="F19">_xlfn.XLOOKUP($A19&amp;F$3&amp;$F$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v>-0.42[-0.74,-0.10]</v>
       </c>
-      <c r="G19" s="9" t="str" cm="1">
+      <c r="G19" s="8" t="str" cm="1">
         <f t="array" ref="G19">_xlfn.XLOOKUP($A19&amp;G$3&amp;$F$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v>-0.37[-0.72,-0.03]</v>
       </c>
-      <c r="H19" s="9" t="str" cm="1">
+      <c r="H19" s="8" t="str" cm="1">
         <f t="array" ref="H19">_xlfn.XLOOKUP($A19&amp;H$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v/>
       </c>
-      <c r="I19" s="9" t="str" cm="1">
+      <c r="I19" s="8" t="str" cm="1">
         <f t="array" ref="I19">_xlfn.XLOOKUP($A19&amp;I$3&amp;$I$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v>-0.70[-1.11,-0.28]</v>
       </c>
-      <c r="J19" s="9" t="str" cm="1">
+      <c r="J19" s="8" t="str" cm="1">
         <f t="array" ref="J19">_xlfn.XLOOKUP($A19&amp;J$3&amp;$I$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
         <v/>
       </c>
-      <c r="O19" s="10"/>
+      <c r="O19" s="9"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
@@ -17759,7 +17758,7 @@
         <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C29" t="str" cm="1">
         <f t="array" ref="C29">_xlfn.XLOOKUP($A29&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -17797,10 +17796,10 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C30" t="str" cm="1">
         <f t="array" ref="C30">_xlfn.XLOOKUP($A30&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -17882,7 +17881,7 @@
         <v>98</v>
       </c>
       <c r="B32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C32" t="str" cm="1">
         <f t="array" ref="C32">_xlfn.XLOOKUP($A32&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -17923,7 +17922,7 @@
         <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C33" t="str" cm="1">
         <f t="array" ref="C33">_xlfn.XLOOKUP($A33&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -17964,7 +17963,7 @@
         <v>105</v>
       </c>
       <c r="B34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C34" t="str" cm="1">
         <f t="array" ref="C34">_xlfn.XLOOKUP($A34&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -18005,7 +18004,7 @@
         <v>107</v>
       </c>
       <c r="B35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C35" t="str" cm="1">
         <f t="array" ref="C35">_xlfn.XLOOKUP($A35&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -18888,7 +18887,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:J35"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19191,7 +19190,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="2" t="str" cm="1">
         <f t="array" ref="C10">_xlfn.XLOOKUP($A10&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -19951,7 +19950,7 @@
         <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C29" t="str" cm="1">
         <f t="array" ref="C29">_xlfn.XLOOKUP($A29&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -19988,10 +19987,10 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C30" t="str" cm="1">
         <f t="array" ref="C30">_xlfn.XLOOKUP($A30&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -20071,7 +20070,7 @@
         <v>98</v>
       </c>
       <c r="B32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C32" t="str" cm="1">
         <f t="array" ref="C32">_xlfn.XLOOKUP($A32&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -20111,7 +20110,7 @@
         <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C33" t="str" cm="1">
         <f t="array" ref="C33">_xlfn.XLOOKUP($A33&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -20151,7 +20150,7 @@
         <v>105</v>
       </c>
       <c r="B34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C34" t="str" cm="1">
         <f t="array" ref="C34">_xlfn.XLOOKUP($A34&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -20191,7 +20190,7 @@
         <v>107</v>
       </c>
       <c r="B35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C35" t="str" cm="1">
         <f t="array" ref="C35">_xlfn.XLOOKUP($A35&amp;C$3&amp;$C$2&amp;$A$1,doses_results!$C$2:$C$400&amp;doses_results!$K$2:$K$400&amp;doses_results!$J$2:$J$400&amp;doses_results!$I$2:$I$400,doses_results!$L$2:$L$400,"",0)</f>
@@ -20279,7 +20278,7 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -21669,7 +21668,7 @@
         <v>ASC_workforce_capacity</v>
       </c>
       <c r="R32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -21984,7 +21983,7 @@
         <v>Core_services_funding_percapita</v>
       </c>
       <c r="R39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -22029,7 +22028,7 @@
         <v>Primary_care_funding_percapita</v>
       </c>
       <c r="R40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
@@ -22074,7 +22073,7 @@
         <v>omicron_support_fund_percapita</v>
       </c>
       <c r="R41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
@@ -27080,10 +27079,10 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C170" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D170">
         <v>0.14847179381960299</v>
@@ -28055,7 +28054,7 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C195" t="s">
         <v>106</v>
@@ -28133,10 +28132,10 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C197" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D197">
         <v>-0.72203732655348196</v>
@@ -28172,7 +28171,7 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C198" t="s">
         <v>107</v>
@@ -28250,7 +28249,7 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C200" t="s">
         <v>108</v>
@@ -28289,7 +28288,7 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C201" t="s">
         <v>109</v>
@@ -28328,7 +28327,7 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C202" t="s">
         <v>110</v>
@@ -29384,7 +29383,7 @@
         <v>18</v>
       </c>
       <c r="C229" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D229">
         <v>1.3904221354439699E-2</v>
@@ -29423,7 +29422,7 @@
         <v>19</v>
       </c>
       <c r="C230" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D230">
         <v>-0.18353646076107999</v>
@@ -29501,7 +29500,7 @@
         <v>21</v>
       </c>
       <c r="C232" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D232">
         <v>3.0157922932812501E-2</v>
@@ -30281,7 +30280,7 @@
         <v>41</v>
       </c>
       <c r="C252" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D252">
         <v>1.1148227686847101</v>
@@ -30320,7 +30319,7 @@
         <v>42</v>
       </c>
       <c r="C253" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D253">
         <v>-10.950594494558199</v>
@@ -30398,7 +30397,7 @@
         <v>44</v>
       </c>
       <c r="C255" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D255">
         <v>-0.52255737774436595</v>
@@ -30641,7 +30640,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:J41"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30903,7 +30902,7 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="8" t="str" cm="1">
         <f t="array" ref="C10">_xlfn.XLOOKUP($A10&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -31549,7 +31548,7 @@
         <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C29" s="8" t="str" cm="1">
         <f t="array" ref="C29">_xlfn.XLOOKUP($A29&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -31583,7 +31582,7 @@
         <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C30" s="8" t="str" cm="1">
         <f t="array" ref="C30">_xlfn.XLOOKUP($A30&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -31617,7 +31616,7 @@
         <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C31" s="8" t="str" cm="1">
         <f t="array" ref="C31">_xlfn.XLOOKUP($A31&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -31648,10 +31647,10 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C32" s="8" t="str" cm="1">
         <f t="array" ref="C32">_xlfn.XLOOKUP($A32&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -31685,7 +31684,7 @@
         <v>107</v>
       </c>
       <c r="B33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C33" s="8" t="str" cm="1">
         <f t="array" ref="C33">_xlfn.XLOOKUP($A33&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -31719,7 +31718,7 @@
         <v>98</v>
       </c>
       <c r="B34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C34" s="8" t="str" cm="1">
         <f t="array" ref="C34">_xlfn.XLOOKUP($A34&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -31753,7 +31752,7 @@
         <v>108</v>
       </c>
       <c r="B35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C35" s="8" t="str" cm="1">
         <f t="array" ref="C35">_xlfn.XLOOKUP($A35&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -31787,7 +31786,7 @@
         <v>109</v>
       </c>
       <c r="B36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C36" s="8" t="str" cm="1">
         <f t="array" ref="C36">_xlfn.XLOOKUP($A36&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -31821,7 +31820,7 @@
         <v>110</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C37" s="8" t="str" cm="1">
         <f t="array" ref="C37">_xlfn.XLOOKUP($A37&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -31886,10 +31885,10 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C39" s="8" t="str" cm="1">
         <f t="array" ref="C39">_xlfn.XLOOKUP($A39&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -31920,10 +31919,10 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C40" s="8" t="str" cm="1">
         <f t="array" ref="C40">_xlfn.XLOOKUP($A40&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -31954,10 +31953,10 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C41" s="8" t="str" cm="1">
         <f t="array" ref="C41">_xlfn.XLOOKUP($A41&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -31998,8 +31997,8 @@
   </sheetPr>
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:J41"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32062,34 +32061,34 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C4" s="9" t="str" cm="1">
+      <c r="C4" s="8" t="str" cm="1">
         <f t="array" ref="C4">_xlfn.XLOOKUP($A4&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>-0.93[-1.36,-0.51]</v>
       </c>
-      <c r="D4" s="9" t="str" cm="1">
+      <c r="D4" s="8" t="str" cm="1">
         <f t="array" ref="D4">_xlfn.XLOOKUP($A4&amp;D$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>-0.82[-1.24,-0.39]</v>
       </c>
-      <c r="F4" s="9" t="str" cm="1">
+      <c r="F4" s="8" t="str" cm="1">
         <f t="array" ref="F4">_xlfn.XLOOKUP($A4&amp;F$3&amp;$F$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>-1.03[-1.44,-0.61]</v>
       </c>
-      <c r="G4" s="9" t="str" cm="1">
+      <c r="G4" s="8" t="str" cm="1">
         <f t="array" ref="G4">_xlfn.XLOOKUP($A4&amp;G$3&amp;$F$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>-0.95[-1.37,-0.54]</v>
       </c>
-      <c r="I4" s="9" t="str" cm="1">
+      <c r="I4" s="8" t="str" cm="1">
         <f t="array" ref="I4">_xlfn.XLOOKUP($A4&amp;I$3&amp;$I$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>12.48[-0.21,25.16]</v>
       </c>
-      <c r="J4" s="9" t="str" cm="1">
+      <c r="J4" s="8" t="str" cm="1">
         <f t="array" ref="J4">_xlfn.XLOOKUP($A4&amp;J$3&amp;$I$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>8.39[-4.05,20.84]</v>
       </c>
@@ -32269,7 +32268,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="5" t="str" cm="1">
         <f t="array" ref="C10">_xlfn.XLOOKUP($A10&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -32502,34 +32501,34 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+    <row r="17" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="9" t="str" cm="1">
+      <c r="C17" s="8" t="str" cm="1">
         <f t="array" ref="C17">_xlfn.XLOOKUP($A17&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>0.29[0.01,0.58]</v>
       </c>
-      <c r="D17" s="9" t="str" cm="1">
+      <c r="D17" s="8" t="str" cm="1">
         <f t="array" ref="D17">_xlfn.XLOOKUP($A17&amp;D$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>0.26[-0.02,0.54]</v>
       </c>
-      <c r="F17" s="9" t="str" cm="1">
+      <c r="F17" s="8" t="str" cm="1">
         <f t="array" ref="F17">_xlfn.XLOOKUP($A17&amp;F$3&amp;$F$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>0.30[0.02,0.59]</v>
       </c>
-      <c r="G17" s="9" t="str" cm="1">
+      <c r="G17" s="8" t="str" cm="1">
         <f t="array" ref="G17">_xlfn.XLOOKUP($A17&amp;G$3&amp;$F$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>0.27[-0.01,0.56]</v>
       </c>
-      <c r="I17" s="9" t="str" cm="1">
+      <c r="I17" s="8" t="str" cm="1">
         <f t="array" ref="I17">_xlfn.XLOOKUP($A17&amp;I$3&amp;$I$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>0.59[-0.95,2.12]</v>
       </c>
-      <c r="J17" s="9" t="str" cm="1">
+      <c r="J17" s="8" t="str" cm="1">
         <f t="array" ref="J17">_xlfn.XLOOKUP($A17&amp;J$3&amp;$I$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>0.37[-1.24,1.98]</v>
       </c>
@@ -32807,35 +32806,35 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C26" s="9" t="str" cm="1">
+      <c r="C26" s="8" t="str" cm="1">
         <f t="array" ref="C26">_xlfn.XLOOKUP($A26&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>0.49[0.19,0.80]</v>
       </c>
-      <c r="D26" s="9" t="str" cm="1">
+      <c r="D26" s="8" t="str" cm="1">
         <f t="array" ref="D26">_xlfn.XLOOKUP($A26&amp;D$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>0.36[0.04,0.68]</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9" t="str" cm="1">
+      <c r="E26" s="8"/>
+      <c r="F26" s="8" t="str" cm="1">
         <f t="array" ref="F26">_xlfn.XLOOKUP($A26&amp;F$3&amp;$F$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>0.15[-0.10,0.40]</v>
       </c>
-      <c r="G26" s="9" t="str" cm="1">
+      <c r="G26" s="8" t="str" cm="1">
         <f t="array" ref="G26">_xlfn.XLOOKUP($A26&amp;G$3&amp;$F$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>0.09[-0.18,0.36]</v>
       </c>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9" t="str" cm="1">
+      <c r="H26" s="8"/>
+      <c r="I26" s="8" t="str" cm="1">
         <f t="array" ref="I26">_xlfn.XLOOKUP($A26&amp;I$3&amp;$I$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>0.33[0.12,0.54]</v>
       </c>
-      <c r="J26" s="9" t="str" cm="1">
+      <c r="J26" s="8" t="str" cm="1">
         <f t="array" ref="J26">_xlfn.XLOOKUP($A26&amp;J$3&amp;$I$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
         <v>0.17[-0.06,0.40]</v>
       </c>
@@ -32913,7 +32912,7 @@
         <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C29" s="8" t="str" cm="1">
         <f t="array" ref="C29">_xlfn.XLOOKUP($A29&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -32947,7 +32946,7 @@
         <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C30" s="8" t="str" cm="1">
         <f t="array" ref="C30">_xlfn.XLOOKUP($A30&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -32981,7 +32980,7 @@
         <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C31" s="8" t="str" cm="1">
         <f t="array" ref="C31">_xlfn.XLOOKUP($A31&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -33012,10 +33011,10 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C32" s="8" t="str" cm="1">
         <f t="array" ref="C32">_xlfn.XLOOKUP($A32&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -33049,7 +33048,7 @@
         <v>107</v>
       </c>
       <c r="B33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C33" s="8" t="str" cm="1">
         <f t="array" ref="C33">_xlfn.XLOOKUP($A33&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -33083,7 +33082,7 @@
         <v>98</v>
       </c>
       <c r="B34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C34" s="8" t="str" cm="1">
         <f t="array" ref="C34">_xlfn.XLOOKUP($A34&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -33117,7 +33116,7 @@
         <v>108</v>
       </c>
       <c r="B35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C35" s="8" t="str" cm="1">
         <f t="array" ref="C35">_xlfn.XLOOKUP($A35&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -33151,7 +33150,7 @@
         <v>109</v>
       </c>
       <c r="B36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C36" s="8" t="str" cm="1">
         <f t="array" ref="C36">_xlfn.XLOOKUP($A36&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -33185,7 +33184,7 @@
         <v>110</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C37" s="8" t="str" cm="1">
         <f t="array" ref="C37">_xlfn.XLOOKUP($A37&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -33250,10 +33249,10 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C39" s="8" t="str" cm="1">
         <f t="array" ref="C39">_xlfn.XLOOKUP($A39&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -33284,10 +33283,10 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C40" s="8" t="str" cm="1">
         <f t="array" ref="C40">_xlfn.XLOOKUP($A40&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>
@@ -33318,10 +33317,10 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C41" s="8" t="str" cm="1">
         <f t="array" ref="C41">_xlfn.XLOOKUP($A41&amp;C$3&amp;$C$2&amp;$A$1,dropout_results!$C$2:$C$300&amp;dropout_results!$K$2:$K$300&amp;dropout_results!$J$2:$J$300&amp;dropout_results!$I$2:$I$300,dropout_results!$L$2:$L$300,"",0)</f>

</xml_diff>